<commit_message>
forecast manual single fixed
</commit_message>
<xml_diff>
--- a/inst/app_demo/HPFC/manual/manual_fwd_gas.xlsx
+++ b/inst/app_demo/HPFC/manual/manual_fwd_gas.xlsx
@@ -1,29 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CG13879\Documents\GitHub\HPFC\HPFC-Package\inst\app_demo\HPFC\manual\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F7C807-1764-44C9-8490-332C901B6FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TTF" sheetId="1" r:id="rId1"/>
+    <sheet name="PSV" sheetId="2" r:id="rId2"/>
+    <sheet name="NBP" sheetId="3" r:id="rId3"/>
+    <sheet name="NCG" sheetId="4" r:id="rId4"/>
+    <sheet name="BRM" sheetId="5" r:id="rId5"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="4">
   <si>
-    <t xml:space="preserve">sim</t>
+    <t>sim</t>
   </si>
   <si>
-    <t xml:space="preserve">yymm</t>
+    <t>yymm</t>
   </si>
   <si>
-    <t xml:space="preserve">value</t>
+    <t>value</t>
   </si>
   <si>
-    <t xml:space="preserve">FWD</t>
+    <t>FWD</t>
   </si>
 </sst>
 </file>
@@ -31,9 +43,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -69,12 +81,21 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -356,14 +377,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,140 +397,775 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="1">
         <v>45292</v>
       </c>
-      <c r="C2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="1">
         <v>45323</v>
       </c>
-      <c r="C3" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>45352</v>
       </c>
-      <c r="C4" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>45383</v>
       </c>
-      <c r="C5" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="1">
         <v>45413</v>
       </c>
-      <c r="C6" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="1">
         <v>45444</v>
       </c>
-      <c r="C7" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>45474</v>
       </c>
-      <c r="C8" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="C8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="1">
         <v>45505</v>
       </c>
-      <c r="C9" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="C9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="1">
         <v>45536</v>
       </c>
-      <c r="C10" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="C10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="1">
         <v>45566</v>
       </c>
-      <c r="C11" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="C11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="1">
         <v>45597</v>
       </c>
-      <c r="C12" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="C12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" s="1">
         <v>45627</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134EF4BB-F6AF-4779-99D2-74AEBC94A2A5}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45292</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45323</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45352</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45413</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45444</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45474</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45505</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45536</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45566</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45597</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45627</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D8B339-89A5-4C89-85E8-88302DD5E66E}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45292</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45323</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45352</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45413</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45444</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45474</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45505</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45536</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45566</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45597</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45627</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D5A7B0-9C86-47B2-8003-27158280AC5E}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45292</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45323</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45352</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45413</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45444</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45474</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45505</v>
+      </c>
+      <c r="C9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45536</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45566</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45597</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45627</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76B220B-890F-4699-829A-AA5AA214C0C6}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45292</v>
+      </c>
+      <c r="C2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45323</v>
+      </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45352</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45383</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45413</v>
+      </c>
+      <c r="C6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45444</v>
+      </c>
+      <c r="C7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45474</v>
+      </c>
+      <c r="C8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45505</v>
+      </c>
+      <c r="C9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45536</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45566</v>
+      </c>
+      <c r="C11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45597</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45627</v>
+      </c>
+      <c r="C13">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>